<commit_message>
Ajout de l'ActionBar pour toutes les version :). Nouveaux logo d'application.
</commit_message>
<xml_diff>
--- a/docs/CRA.xlsx
+++ b/docs/CRA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>taches</t>
   </si>
@@ -50,6 +50,10 @@
   </si>
   <si>
     <t>Débuggage eclipse android mac</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActionBar all version !</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -426,7 +430,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -494,18 +498,30 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6">
+        <v>41064</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1">
         <f>SUM(B2:B15)</f>
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Refresh button + progressbar
</commit_message>
<xml_diff>
--- a/docs/CRA.xlsx
+++ b/docs/CRA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>taches</t>
   </si>
@@ -54,6 +54,10 @@
   </si>
   <si>
     <t>ActionBar all version !</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No pull on refresh but a refresh button with actionView !</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -430,7 +434,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -509,19 +513,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6">
+        <v>41065</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1">
         <f>SUM(B2:B15)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>